<commit_message>
Write clean subplot data, including fixes made from looking at scanned data sheets
</commit_message>
<xml_diff>
--- a/data/data-wrangling-intermediate/04.1b_edited7_NA-count-of-non-0-Code-corrected.xlsx
+++ b/data/data-wrangling-intermediate/04.1b_edited7_NA-count-of-non-0-Code-corrected.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://emailarizona-my.sharepoint.com/personal/lossanna_arizona_edu/Documents/grad school/Gornish lab/04_RAMPS RestoreNet/RestoreNet/data/data-wrangling-intermediate/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{031DDA90-BC7D-497D-9D67-BD23FE43E6B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="45" documentId="13_ncr:40009_{031DDA90-BC7D-497D-9D67-BD23FE43E6B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F645FD02-CA9C-4F8D-8852-AEE0A0035449}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15270"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="04.1b_edited7_NA-count-of-non-0" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="81">
   <si>
     <t>Region</t>
   </si>
@@ -116,9 +116,6 @@
   </si>
   <si>
     <t>Grass</t>
-  </si>
-  <si>
-    <t>NA</t>
   </si>
   <si>
     <t>No</t>
@@ -271,8 +268,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -403,6 +400,12 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -755,10 +758,14 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -828,9 +835,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>502920</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>45720</xdr:rowOff>
+      <xdr:colOff>506730</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -845,8 +852,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7239000" y="2758440"/>
-          <a:ext cx="3627120" cy="762000"/>
+          <a:off x="7934325" y="2729865"/>
+          <a:ext cx="3630930" cy="1013460"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -886,19 +893,31 @@
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t> Count and Height (if applicable) columns by looking back at scans of hard-copy raw data sheets.</a:t>
+            <a:t> Count and Height (if applicable) columns by looking back at scans of hard-copy raw data sheets. NAs changed to blank cells.</a:t>
           </a:r>
-          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Red</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> = scanned data sheet not available</a:t>
+          </a:r>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1217,11 +1236,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1277,7 +1296,7 @@
       <c r="O1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="P1" t="s">
         <v>15</v>
       </c>
       <c r="Q1" t="s">
@@ -1303,19 +1322,19 @@
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="3">
         <v>43404</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="3">
         <v>43594</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="2">
         <v>175</v>
       </c>
       <c r="F2">
@@ -1349,64 +1368,61 @@
         <v>31</v>
       </c>
       <c r="P2" s="2"/>
-      <c r="Q2" t="s">
-        <v>32</v>
-      </c>
       <c r="R2">
         <v>10842</v>
       </c>
       <c r="S2" t="s">
+        <v>32</v>
+      </c>
+      <c r="T2" t="s">
         <v>33</v>
       </c>
-      <c r="T2" t="s">
-        <v>34</v>
-      </c>
       <c r="U2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="V2" t="s">
         <v>21</v>
       </c>
       <c r="W2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C3" s="1">
+      <c r="B3" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" s="3">
         <v>43390</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="3">
         <v>43602</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="2">
         <v>167</v>
       </c>
       <c r="F3">
         <v>18</v>
       </c>
       <c r="G3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H3" t="s">
         <v>37</v>
-      </c>
-      <c r="H3" t="s">
-        <v>38</v>
       </c>
       <c r="I3">
         <v>4268</v>
       </c>
       <c r="J3" t="s">
+        <v>38</v>
+      </c>
+      <c r="K3" t="s">
+        <v>38</v>
+      </c>
+      <c r="L3" t="s">
         <v>39</v>
-      </c>
-      <c r="K3" t="s">
-        <v>39</v>
-      </c>
-      <c r="L3" t="s">
-        <v>40</v>
       </c>
       <c r="M3" t="s">
         <v>29</v>
@@ -1415,138 +1431,133 @@
         <v>30</v>
       </c>
       <c r="O3" t="s">
-        <v>41</v>
-      </c>
-      <c r="P3" s="2">
-        <v>3</v>
-      </c>
-      <c r="Q3" s="2">
-        <v>120</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="P3" s="2"/>
       <c r="R3">
         <v>11297</v>
       </c>
       <c r="S3" t="s">
+        <v>32</v>
+      </c>
+      <c r="T3" t="s">
         <v>33</v>
       </c>
-      <c r="T3" t="s">
-        <v>34</v>
-      </c>
       <c r="U3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="V3" t="s">
         <v>21</v>
       </c>
       <c r="W3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C4" s="1">
+      <c r="C4" s="5">
         <v>44048</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="5">
         <v>44479</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="4">
         <v>13</v>
       </c>
       <c r="F4">
         <v>218</v>
       </c>
       <c r="G4" t="s">
+        <v>36</v>
+      </c>
+      <c r="H4" t="s">
         <v>37</v>
-      </c>
-      <c r="H4" t="s">
-        <v>38</v>
       </c>
       <c r="I4">
         <v>6143</v>
       </c>
       <c r="J4" t="s">
+        <v>43</v>
+      </c>
+      <c r="K4" t="s">
+        <v>43</v>
+      </c>
+      <c r="L4" t="s">
         <v>44</v>
-      </c>
-      <c r="K4" t="s">
-        <v>44</v>
-      </c>
-      <c r="L4" t="s">
-        <v>45</v>
       </c>
       <c r="M4" t="s">
         <v>12</v>
       </c>
       <c r="N4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="O4" t="s">
-        <v>41</v>
-      </c>
-      <c r="P4" s="2"/>
-      <c r="Q4">
+        <v>40</v>
+      </c>
+      <c r="P4" s="6">
         <v>125</v>
       </c>
+      <c r="Q4" s="1"/>
       <c r="R4">
         <v>16798</v>
       </c>
       <c r="S4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="T4" t="s">
+        <v>46</v>
+      </c>
+      <c r="U4" t="s">
         <v>47</v>
       </c>
-      <c r="U4" t="s">
+      <c r="V4" t="s">
         <v>48</v>
       </c>
-      <c r="V4" t="s">
-        <v>49</v>
-      </c>
       <c r="W4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C5" s="1">
+      <c r="C5" s="5">
         <v>44048</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="5">
         <v>44479</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="4">
         <v>13</v>
       </c>
       <c r="F5">
         <v>222</v>
       </c>
       <c r="G5" t="s">
+        <v>49</v>
+      </c>
+      <c r="H5" t="s">
         <v>50</v>
-      </c>
-      <c r="H5" t="s">
-        <v>51</v>
       </c>
       <c r="I5">
         <v>6147</v>
       </c>
       <c r="J5" t="s">
+        <v>51</v>
+      </c>
+      <c r="K5" t="s">
+        <v>51</v>
+      </c>
+      <c r="L5" t="s">
         <v>52</v>
-      </c>
-      <c r="K5" t="s">
-        <v>52</v>
-      </c>
-      <c r="L5" t="s">
-        <v>53</v>
       </c>
       <c r="M5" t="s">
         <v>12</v>
@@ -1555,136 +1566,136 @@
         <v>30</v>
       </c>
       <c r="O5" t="s">
-        <v>41</v>
-      </c>
-      <c r="P5" s="2"/>
-      <c r="Q5">
+        <v>40</v>
+      </c>
+      <c r="P5" s="1">
         <v>230</v>
       </c>
+      <c r="Q5" s="1"/>
       <c r="R5">
         <v>16810</v>
       </c>
       <c r="S5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="T5" t="s">
+        <v>46</v>
+      </c>
+      <c r="U5" t="s">
         <v>47</v>
       </c>
-      <c r="U5" t="s">
+      <c r="V5" t="s">
         <v>48</v>
       </c>
-      <c r="V5" t="s">
-        <v>49</v>
-      </c>
       <c r="W5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B6" t="s">
-        <v>43</v>
-      </c>
-      <c r="C6" s="1">
+      <c r="C6" s="5">
         <v>44048</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" s="5">
         <v>44479</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="4">
         <v>13</v>
       </c>
       <c r="F6">
         <v>222</v>
       </c>
       <c r="G6" t="s">
+        <v>49</v>
+      </c>
+      <c r="H6" t="s">
         <v>50</v>
-      </c>
-      <c r="H6" t="s">
-        <v>51</v>
       </c>
       <c r="I6">
         <v>6147</v>
       </c>
       <c r="J6" t="s">
+        <v>43</v>
+      </c>
+      <c r="K6" t="s">
+        <v>43</v>
+      </c>
+      <c r="L6" t="s">
         <v>44</v>
-      </c>
-      <c r="K6" t="s">
-        <v>44</v>
-      </c>
-      <c r="L6" t="s">
-        <v>45</v>
       </c>
       <c r="M6" t="s">
         <v>12</v>
       </c>
       <c r="N6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="O6" t="s">
-        <v>41</v>
-      </c>
-      <c r="P6" s="2"/>
-      <c r="Q6">
+        <v>40</v>
+      </c>
+      <c r="P6" s="1">
         <v>275</v>
       </c>
+      <c r="Q6" s="1"/>
       <c r="R6">
         <v>16811</v>
       </c>
       <c r="S6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="T6" t="s">
+        <v>46</v>
+      </c>
+      <c r="U6" t="s">
         <v>47</v>
       </c>
-      <c r="U6" t="s">
+      <c r="V6" t="s">
         <v>48</v>
       </c>
-      <c r="V6" t="s">
-        <v>49</v>
-      </c>
       <c r="W6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="A7" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B7" t="s">
-        <v>43</v>
-      </c>
-      <c r="C7" s="1">
+      <c r="C7" s="5">
         <v>44048</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7" s="5">
         <v>44479</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="4">
         <v>13</v>
       </c>
       <c r="F7">
         <v>222</v>
       </c>
       <c r="G7" t="s">
+        <v>49</v>
+      </c>
+      <c r="H7" t="s">
         <v>50</v>
-      </c>
-      <c r="H7" t="s">
-        <v>51</v>
       </c>
       <c r="I7">
         <v>6147</v>
       </c>
       <c r="J7" t="s">
+        <v>54</v>
+      </c>
+      <c r="K7" t="s">
+        <v>54</v>
+      </c>
+      <c r="L7" t="s">
         <v>55</v>
-      </c>
-      <c r="K7" t="s">
-        <v>55</v>
-      </c>
-      <c r="L7" t="s">
-        <v>56</v>
       </c>
       <c r="M7" t="s">
         <v>12</v>
@@ -1695,134 +1706,134 @@
       <c r="O7" t="s">
         <v>31</v>
       </c>
-      <c r="P7" s="2"/>
-      <c r="Q7">
+      <c r="P7" s="1">
         <v>210</v>
       </c>
+      <c r="Q7" s="1"/>
       <c r="R7">
         <v>16812</v>
       </c>
       <c r="S7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="T7" t="s">
+        <v>46</v>
+      </c>
+      <c r="U7" t="s">
         <v>47</v>
       </c>
-      <c r="U7" t="s">
+      <c r="V7" t="s">
         <v>48</v>
       </c>
-      <c r="V7" t="s">
-        <v>49</v>
-      </c>
       <c r="W7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="A8" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B8" t="s">
-        <v>43</v>
-      </c>
-      <c r="C8" s="1">
+      <c r="C8" s="5">
         <v>44048</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8" s="5">
         <v>44479</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="4">
         <v>13</v>
       </c>
       <c r="F8">
         <v>222</v>
       </c>
       <c r="G8" t="s">
+        <v>49</v>
+      </c>
+      <c r="H8" t="s">
         <v>50</v>
-      </c>
-      <c r="H8" t="s">
-        <v>51</v>
       </c>
       <c r="I8">
         <v>6147</v>
       </c>
       <c r="J8" t="s">
+        <v>56</v>
+      </c>
+      <c r="K8" t="s">
+        <v>56</v>
+      </c>
+      <c r="L8" t="s">
         <v>57</v>
-      </c>
-      <c r="K8" t="s">
-        <v>57</v>
-      </c>
-      <c r="L8" t="s">
-        <v>58</v>
       </c>
       <c r="M8" t="s">
         <v>12</v>
       </c>
       <c r="N8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="O8" t="s">
-        <v>41</v>
-      </c>
-      <c r="P8" s="2"/>
-      <c r="Q8">
+        <v>40</v>
+      </c>
+      <c r="P8" s="1">
         <v>90</v>
       </c>
+      <c r="Q8" s="1"/>
       <c r="R8">
         <v>16813</v>
       </c>
       <c r="S8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="T8" t="s">
+        <v>46</v>
+      </c>
+      <c r="U8" t="s">
         <v>47</v>
       </c>
-      <c r="U8" t="s">
+      <c r="V8" t="s">
         <v>48</v>
       </c>
-      <c r="V8" t="s">
-        <v>49</v>
-      </c>
       <c r="W8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="A9" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B9" t="s">
-        <v>43</v>
-      </c>
-      <c r="C9" s="1">
+      <c r="C9" s="5">
         <v>44048</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9" s="5">
         <v>44479</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="4">
         <v>13</v>
       </c>
       <c r="F9">
         <v>222</v>
       </c>
       <c r="G9" t="s">
+        <v>49</v>
+      </c>
+      <c r="H9" t="s">
         <v>50</v>
-      </c>
-      <c r="H9" t="s">
-        <v>51</v>
       </c>
       <c r="I9">
         <v>6147</v>
       </c>
       <c r="J9" t="s">
+        <v>59</v>
+      </c>
+      <c r="K9" t="s">
+        <v>59</v>
+      </c>
+      <c r="L9" t="s">
         <v>60</v>
-      </c>
-      <c r="K9" t="s">
-        <v>60</v>
-      </c>
-      <c r="L9" t="s">
-        <v>61</v>
       </c>
       <c r="M9" t="s">
         <v>12</v>
@@ -1831,136 +1842,136 @@
         <v>30</v>
       </c>
       <c r="O9" t="s">
-        <v>41</v>
-      </c>
-      <c r="P9" s="2"/>
-      <c r="Q9">
+        <v>40</v>
+      </c>
+      <c r="P9" s="1">
         <v>117</v>
       </c>
+      <c r="Q9" s="1"/>
       <c r="R9">
         <v>16814</v>
       </c>
       <c r="S9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="T9" t="s">
+        <v>46</v>
+      </c>
+      <c r="U9" t="s">
         <v>47</v>
       </c>
-      <c r="U9" t="s">
+      <c r="V9" t="s">
         <v>48</v>
       </c>
-      <c r="V9" t="s">
-        <v>49</v>
-      </c>
       <c r="W9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="A10" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B10" t="s">
-        <v>43</v>
-      </c>
-      <c r="C10" s="1">
+      <c r="C10" s="5">
         <v>44048</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D10" s="5">
         <v>44479</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="4">
         <v>13</v>
       </c>
       <c r="F10">
         <v>222</v>
       </c>
       <c r="G10" t="s">
+        <v>49</v>
+      </c>
+      <c r="H10" t="s">
         <v>50</v>
-      </c>
-      <c r="H10" t="s">
-        <v>51</v>
       </c>
       <c r="I10">
         <v>6147</v>
       </c>
       <c r="J10" t="s">
+        <v>61</v>
+      </c>
+      <c r="K10" t="s">
         <v>62</v>
       </c>
-      <c r="K10" t="s">
+      <c r="L10" t="s">
         <v>63</v>
       </c>
-      <c r="L10" t="s">
-        <v>64</v>
-      </c>
       <c r="M10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="O10" t="s">
         <v>31</v>
       </c>
-      <c r="P10" s="2"/>
-      <c r="Q10">
+      <c r="P10" s="1">
         <v>130</v>
       </c>
+      <c r="Q10" s="1"/>
       <c r="R10">
         <v>16815</v>
       </c>
       <c r="S10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="T10" t="s">
+        <v>64</v>
+      </c>
+      <c r="U10" t="s">
         <v>65</v>
-      </c>
-      <c r="U10" t="s">
-        <v>66</v>
       </c>
       <c r="V10" t="s">
         <v>21</v>
       </c>
       <c r="W10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="A11" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" s="3">
+        <v>43791</v>
+      </c>
+      <c r="D11" s="3">
+        <v>44648</v>
+      </c>
+      <c r="E11" s="2">
+        <v>135</v>
+      </c>
+      <c r="F11" s="2">
+        <v>26</v>
+      </c>
+      <c r="G11" t="s">
         <v>68</v>
       </c>
-      <c r="C11" s="1">
-        <v>43791</v>
-      </c>
-      <c r="D11" s="1">
-        <v>44648</v>
-      </c>
-      <c r="E11">
-        <v>135</v>
-      </c>
-      <c r="F11">
-        <v>26</v>
-      </c>
-      <c r="G11" t="s">
-        <v>69</v>
-      </c>
       <c r="H11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I11">
         <v>6259</v>
       </c>
       <c r="J11" t="s">
+        <v>69</v>
+      </c>
+      <c r="K11" t="s">
+        <v>69</v>
+      </c>
+      <c r="L11" t="s">
         <v>70</v>
-      </c>
-      <c r="K11" t="s">
-        <v>70</v>
-      </c>
-      <c r="L11" t="s">
-        <v>71</v>
       </c>
       <c r="M11" t="s">
         <v>29</v>
@@ -1979,57 +1990,57 @@
         <v>17607</v>
       </c>
       <c r="S11" t="s">
+        <v>32</v>
+      </c>
+      <c r="T11" t="s">
         <v>33</v>
       </c>
-      <c r="T11" t="s">
-        <v>34</v>
-      </c>
       <c r="U11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="V11" t="s">
         <v>21</v>
       </c>
       <c r="W11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="A12" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B12" t="s">
-        <v>73</v>
-      </c>
-      <c r="C12" s="1">
+      <c r="C12" s="3">
         <v>44578</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D12" s="3">
         <v>44664</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="2">
         <v>117</v>
       </c>
       <c r="F12">
         <v>18</v>
       </c>
       <c r="G12" t="s">
+        <v>36</v>
+      </c>
+      <c r="H12" t="s">
         <v>37</v>
-      </c>
-      <c r="H12" t="s">
-        <v>38</v>
       </c>
       <c r="I12">
         <v>6286</v>
       </c>
       <c r="J12" t="s">
+        <v>73</v>
+      </c>
+      <c r="K12" t="s">
         <v>74</v>
       </c>
-      <c r="K12" t="s">
+      <c r="L12" t="s">
         <v>75</v>
-      </c>
-      <c r="L12" t="s">
-        <v>76</v>
       </c>
       <c r="M12" t="s">
         <v>12</v>
@@ -2038,67 +2049,64 @@
         <v>30</v>
       </c>
       <c r="O12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="P12" s="2"/>
-      <c r="Q12" t="s">
-        <v>32</v>
-      </c>
       <c r="R12">
         <v>17737</v>
       </c>
       <c r="S12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="T12" t="s">
+        <v>46</v>
+      </c>
+      <c r="U12" t="s">
         <v>47</v>
       </c>
-      <c r="U12" t="s">
+      <c r="V12" t="s">
         <v>48</v>
       </c>
-      <c r="V12" t="s">
-        <v>49</v>
-      </c>
       <c r="W12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="A13" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B13" t="s">
-        <v>73</v>
-      </c>
-      <c r="C13" s="1">
+      <c r="C13" s="3">
         <v>44578</v>
       </c>
-      <c r="D13" s="1">
+      <c r="D13" s="3">
         <v>44664</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="2">
         <v>117</v>
       </c>
       <c r="F13">
         <v>18</v>
       </c>
       <c r="G13" t="s">
+        <v>36</v>
+      </c>
+      <c r="H13" t="s">
         <v>37</v>
-      </c>
-      <c r="H13" t="s">
-        <v>38</v>
       </c>
       <c r="I13">
         <v>6286</v>
       </c>
       <c r="J13" t="s">
+        <v>76</v>
+      </c>
+      <c r="K13" t="s">
+        <v>76</v>
+      </c>
+      <c r="L13" t="s">
         <v>77</v>
-      </c>
-      <c r="K13" t="s">
-        <v>77</v>
-      </c>
-      <c r="L13" t="s">
-        <v>78</v>
       </c>
       <c r="M13" t="s">
         <v>29</v>
@@ -2107,45 +2115,42 @@
         <v>30</v>
       </c>
       <c r="O13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="P13" s="2"/>
-      <c r="Q13" t="s">
-        <v>32</v>
-      </c>
       <c r="R13">
         <v>17742</v>
       </c>
       <c r="S13" t="s">
+        <v>32</v>
+      </c>
+      <c r="T13" t="s">
         <v>33</v>
       </c>
-      <c r="T13" t="s">
-        <v>34</v>
-      </c>
       <c r="U13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="V13" t="s">
         <v>21</v>
       </c>
       <c r="W13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="A14" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B14" t="s">
-        <v>73</v>
-      </c>
-      <c r="C14" s="1">
+      <c r="C14" s="3">
         <v>44578</v>
       </c>
-      <c r="D14" s="1">
+      <c r="D14" s="3">
         <v>44664</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="2">
         <v>117</v>
       </c>
       <c r="F14">
@@ -2155,19 +2160,19 @@
         <v>25</v>
       </c>
       <c r="H14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I14">
         <v>6304</v>
       </c>
       <c r="J14" t="s">
+        <v>79</v>
+      </c>
+      <c r="K14" t="s">
+        <v>79</v>
+      </c>
+      <c r="L14" t="s">
         <v>80</v>
-      </c>
-      <c r="K14" t="s">
-        <v>80</v>
-      </c>
-      <c r="L14" t="s">
-        <v>81</v>
       </c>
       <c r="M14" t="s">
         <v>29</v>
@@ -2176,29 +2181,26 @@
         <v>30</v>
       </c>
       <c r="O14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="P14" s="2"/>
-      <c r="Q14" t="s">
-        <v>32</v>
-      </c>
       <c r="R14">
         <v>17822</v>
       </c>
       <c r="S14" t="s">
+        <v>32</v>
+      </c>
+      <c r="T14" t="s">
         <v>33</v>
       </c>
-      <c r="T14" t="s">
-        <v>34</v>
-      </c>
       <c r="U14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="V14" t="s">
         <v>21</v>
       </c>
       <c r="W14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>